<commit_message>
add animation and modal
</commit_message>
<xml_diff>
--- a/react-shopping-cart/Task_management_for_react_shopping_cart_project.xlsx
+++ b/react-shopping-cart/Task_management_for_react_shopping_cart_project.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Features</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -188,7 +185,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,28 +597,28 @@
       </c>
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>41</v>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D6" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D7">
         <v>2</v>

</xml_diff>

<commit_message>
add redux to Filter component
</commit_message>
<xml_diff>
--- a/react-shopping-cart/Task_management_for_react_shopping_cart_project.xlsx
+++ b/react-shopping-cart/Task_management_for_react_shopping_cart_project.xlsx
@@ -500,7 +500,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,65 +642,65 @@
         <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>41</v>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
+      <c r="C10" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>6</v>
+      <c r="C11" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="4">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add redux to cart
</commit_message>
<xml_diff>
--- a/react-shopping-cart/Task_management_for_react_shopping_cart_project.xlsx
+++ b/react-shopping-cart/Task_management_for_react_shopping_cart_project.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Features</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -173,7 +170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,12 +189,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -211,12 +202,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +490,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,7 +524,7 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -555,7 +545,7 @@
       <c r="C3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -578,7 +568,7 @@
       <c r="C4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -602,7 +592,7 @@
       <c r="C5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>3</v>
       </c>
     </row>
@@ -616,7 +606,7 @@
       <c r="C6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>2</v>
       </c>
     </row>
@@ -630,7 +620,7 @@
       <c r="C7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>2</v>
       </c>
     </row>
@@ -644,7 +634,7 @@
       <c r="C8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>2</v>
       </c>
     </row>
@@ -658,7 +648,7 @@
       <c r="C9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>3</v>
       </c>
     </row>
@@ -672,7 +662,7 @@
       <c r="C10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>2</v>
       </c>
     </row>
@@ -686,35 +676,35 @@
       <c r="C11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
+      <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>